<commit_message>
Stream data from archives during DB build
</commit_message>
<xml_diff>
--- a/docs/script-performance-stats.xlsx
+++ b/docs/script-performance-stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\final-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\final-project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41C28C-3961-4528-A0FE-6468695EC04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3086525-8CE2-4891-B248-71CF0CBC4FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7980" yWindow="528" windowWidth="21696" windowHeight="14784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Build DB" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -60,16 +60,19 @@
     <t>Export feature matrix (s)</t>
   </si>
   <si>
-    <t>High-level 1M (max_workers=8)</t>
-  </si>
-  <si>
-    <t>High-level 1M (auto max_workers)</t>
-  </si>
-  <si>
-    <t>High-level 1M (json instead of orjson)</t>
-  </si>
-  <si>
     <t>Sample 100K</t>
+  </si>
+  <si>
+    <t>auto max_workers</t>
+  </si>
+  <si>
+    <t>max_workers=8</t>
+  </si>
+  <si>
+    <t>json instead of orjson</t>
+  </si>
+  <si>
+    <t>archive streaming</t>
   </si>
 </sst>
 </file>
@@ -389,21 +392,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="28.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,16 +417,22 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -436,8 +448,14 @@
       <c r="E2" s="2">
         <v>100000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -453,8 +471,14 @@
       <c r="E3" s="1">
         <v>35.770000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="1">
+        <v>288.83</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2315.3000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -470,8 +494,14 @@
       <c r="E4" s="2">
         <v>10599</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>276601</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1643001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -487,8 +517,14 @@
       <c r="E5" s="2">
         <v>1404</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>26599</v>
+      </c>
+      <c r="G5" s="2">
+        <v>217394</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -504,8 +540,14 @@
       <c r="E6" s="2">
         <v>4551</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>72488</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1575397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -521,8 +563,14 @@
       <c r="E7" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>6.92</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -538,8 +586,14 @@
       <c r="E8" s="2">
         <v>84850</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>650911</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1781602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -555,8 +609,14 @@
       <c r="E9" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="1">
+        <v>75.23</v>
+      </c>
+      <c r="G9" s="1">
+        <v>400.34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -572,8 +632,14 @@
       <c r="E10" s="1">
         <v>6.62</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <v>78.36</v>
+      </c>
+      <c r="G10" s="1">
+        <v>258.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -588,6 +654,12 @@
       </c>
       <c r="E11" s="1">
         <v>0.44</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3.88</v>
+      </c>
+      <c r="G11" s="1">
+        <v>15.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix ingest perf decrease after switching DB engines
</commit_message>
<xml_diff>
--- a/docs/script-performance-stats.xlsx
+++ b/docs/script-performance-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\final-project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3086525-8CE2-4891-B248-71CF0CBC4FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B165CD-2191-4067-B30F-6E2AFEA72FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13236" yWindow="528" windowWidth="17484" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Build DB" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>archive streaming</t>
+  </si>
+  <si>
+    <t>postgres switch</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,10 +409,11 @@
     <col min="4" max="4" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +435,11 @@
       <c r="G1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -454,8 +461,11 @@
       <c r="G2" s="2">
         <v>5000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="2">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -477,8 +487,11 @@
       <c r="G3" s="1">
         <v>2315.3000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="1">
+        <v>1334.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -500,8 +513,11 @@
       <c r="G4" s="2">
         <v>1643001</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="2">
+        <v>2615660</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -523,8 +539,11 @@
       <c r="G5" s="2">
         <v>217394</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="2">
+        <v>341491</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -546,8 +565,11 @@
       <c r="G6" s="2">
         <v>1575397</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="2">
+        <v>69696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -569,8 +591,11 @@
       <c r="G7" s="1">
         <v>8.92</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -592,8 +617,11 @@
       <c r="G8" s="2">
         <v>1781602</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="2">
+        <v>1921455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -615,8 +643,11 @@
       <c r="G9" s="1">
         <v>400.34</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="1">
+        <v>336.06</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -638,8 +669,11 @@
       <c r="G10" s="1">
         <v>258.33</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="1">
+        <v>450.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -660,6 +694,9 @@
       </c>
       <c r="G11" s="1">
         <v>15.37</v>
+      </c>
+      <c r="H11" s="1">
+        <v>25.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>